<commit_message>
More work on 108 Excel
</commit_message>
<xml_diff>
--- a/108-notes.xlsx
+++ b/108-notes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="21">
   <si>
     <t>denominator</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>PRINT IT</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -99,12 +102,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -119,11 +146,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +512,7 @@
         <v>4</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -492,6 +523,7 @@
         <v>5</v>
       </c>
       <c r="F5">
+        <f>F3*F1</f>
         <v>20</v>
       </c>
     </row>
@@ -503,6 +535,7 @@
         <v>7</v>
       </c>
       <c r="F6">
+        <f>F3-F4</f>
         <v>1</v>
       </c>
     </row>
@@ -514,6 +547,7 @@
         <v>9</v>
       </c>
       <c r="F7">
+        <f>F3-F6</f>
         <v>1</v>
       </c>
     </row>
@@ -524,7 +558,8 @@
       <c r="E8" t="s">
         <v>12</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="5">
+        <f>F5/F6</f>
         <v>20</v>
       </c>
     </row>
@@ -535,7 +570,8 @@
       <c r="E9" t="s">
         <v>13</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="5">
+        <f>F5/F7</f>
         <v>20</v>
       </c>
     </row>
@@ -546,16 +582,18 @@
       <c r="E10" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>17</v>
+      <c r="F10" s="1" t="b">
+        <f>IF(MOD(F5,F6)=0,TRUE,FALSE)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>17</v>
+      <c r="F11" s="1" t="b">
+        <f>IF(MOD(F5,F9)=0,TRUE,FALSE)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -568,6 +606,1008 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <f>F17*F15</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20">
+        <f>F17-F18</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21">
+        <f>F17-F20</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="5">
+        <f>F19/F20</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="5">
+        <f>F19/F21</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="1" t="b">
+        <f>IF(MOD(F19,F20)=0,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="1" t="b">
+        <f>IF(MOD(F19,F23)=0,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33">
+        <f>F31*F29</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34">
+        <f>F31-F32</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35">
+        <f>F31-F34</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="2">
+        <f>F33/F34</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="2">
+        <f>F33/F35</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="1" t="b">
+        <f>IF(MOD(F33,F34)=0,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="1" t="b">
+        <f>IF(MOD(F33,F37)=0,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>4</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47">
+        <f>F45*F43</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48">
+        <f>F45-F46</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49">
+        <f>F45-F48</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="3">
+        <f>F47/F48</f>
+        <v>13.333333333333334</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" s="3">
+        <f>F47/F49</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>14</v>
+      </c>
+      <c r="E52" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" s="1" t="b">
+        <f>IF(MOD(F47,F48)=0,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" s="1" t="b">
+        <f>IF(MOD(F47,F51)=0,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>18</v>
+      </c>
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>2</v>
+      </c>
+      <c r="F59">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>4</v>
+      </c>
+      <c r="F60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" t="s">
+        <v>5</v>
+      </c>
+      <c r="F61">
+        <f>F59*F57</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" t="s">
+        <v>7</v>
+      </c>
+      <c r="F62">
+        <f>F59-F60</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63">
+        <f>F59-F62</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" s="2">
+        <f>F61/F62</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="2">
+        <f>F61/F63</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>14</v>
+      </c>
+      <c r="E66" t="s">
+        <v>15</v>
+      </c>
+      <c r="F66" s="1" t="b">
+        <f>IF(MOD(F61,F62)=0,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E67" t="s">
+        <v>16</v>
+      </c>
+      <c r="F67" s="1" t="b">
+        <f>IF(MOD(F61,F65)=0,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
+        <v>18</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E69" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>1</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>2</v>
+      </c>
+      <c r="F73">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>4</v>
+      </c>
+      <c r="F74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>3</v>
+      </c>
+      <c r="E75" t="s">
+        <v>5</v>
+      </c>
+      <c r="F75">
+        <f>F73*F71</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>6</v>
+      </c>
+      <c r="E76" t="s">
+        <v>7</v>
+      </c>
+      <c r="F76">
+        <f>F73-F74</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" t="s">
+        <v>9</v>
+      </c>
+      <c r="F77">
+        <f>F73-F76</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
+        <v>10</v>
+      </c>
+      <c r="E78" t="s">
+        <v>12</v>
+      </c>
+      <c r="F78" s="3">
+        <f>F75/F76</f>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>11</v>
+      </c>
+      <c r="E79" t="s">
+        <v>13</v>
+      </c>
+      <c r="F79" s="3">
+        <f>F75/F77</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>14</v>
+      </c>
+      <c r="E80" t="s">
+        <v>15</v>
+      </c>
+      <c r="F80" s="1" t="b">
+        <f>IF(MOD(F75,F76)=0,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E81" t="s">
+        <v>16</v>
+      </c>
+      <c r="F81" s="1" t="b">
+        <f>IF(MOD(F75,F79)=0,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E82" t="s">
+        <v>18</v>
+      </c>
+      <c r="F82" s="1"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E83" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>1</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>2</v>
+      </c>
+      <c r="F87">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>4</v>
+      </c>
+      <c r="F88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
+        <v>3</v>
+      </c>
+      <c r="E89" t="s">
+        <v>5</v>
+      </c>
+      <c r="F89">
+        <f>F87*F85</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
+        <v>6</v>
+      </c>
+      <c r="E90" t="s">
+        <v>7</v>
+      </c>
+      <c r="F90">
+        <f>F87-F88</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>8</v>
+      </c>
+      <c r="E91" t="s">
+        <v>9</v>
+      </c>
+      <c r="F91">
+        <f>F87-F90</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
+        <v>10</v>
+      </c>
+      <c r="E92" t="s">
+        <v>12</v>
+      </c>
+      <c r="F92" s="3">
+        <f>F89/F90</f>
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
+        <v>11</v>
+      </c>
+      <c r="E93" t="s">
+        <v>13</v>
+      </c>
+      <c r="F93" s="3">
+        <f>F89/F91</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>14</v>
+      </c>
+      <c r="E94" t="s">
+        <v>15</v>
+      </c>
+      <c r="F94" s="1" t="b">
+        <f>IF(MOD(F89,F90)=0,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E95" t="s">
+        <v>16</v>
+      </c>
+      <c r="F95" s="1" t="b">
+        <f>IF(MOD(F89,F93)=0,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E96" t="s">
+        <v>18</v>
+      </c>
+      <c r="F96" s="1"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E97" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>0</v>
+      </c>
+      <c r="F99">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>1</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>2</v>
+      </c>
+      <c r="F101">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C102" t="s">
+        <v>4</v>
+      </c>
+      <c r="F102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>3</v>
+      </c>
+      <c r="E103" t="s">
+        <v>5</v>
+      </c>
+      <c r="F103">
+        <f>F101*F99</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
+        <v>6</v>
+      </c>
+      <c r="E104" t="s">
+        <v>7</v>
+      </c>
+      <c r="F104">
+        <f>F101-F102</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D105" t="s">
+        <v>8</v>
+      </c>
+      <c r="E105" t="s">
+        <v>9</v>
+      </c>
+      <c r="F105">
+        <f>F101-F104</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
+        <v>10</v>
+      </c>
+      <c r="E106" t="s">
+        <v>12</v>
+      </c>
+      <c r="F106" s="4">
+        <f>F103/F104</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
+        <v>11</v>
+      </c>
+      <c r="E107" t="s">
+        <v>13</v>
+      </c>
+      <c r="F107" s="4">
+        <f>F103/F105</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D108" t="s">
+        <v>14</v>
+      </c>
+      <c r="E108" t="s">
+        <v>15</v>
+      </c>
+      <c r="F108" s="1" t="b">
+        <f>IF(MOD(F103,F104)=0,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E109" t="s">
+        <v>16</v>
+      </c>
+      <c r="F109" s="1" t="b">
+        <f>IF(MOD(F103,F107)=0,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E110" t="s">
+        <v>18</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E111" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>0</v>
+      </c>
+      <c r="F113">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>1</v>
+      </c>
+      <c r="F114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>2</v>
+      </c>
+      <c r="F115">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C116" t="s">
+        <v>4</v>
+      </c>
+      <c r="F116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D117" t="s">
+        <v>3</v>
+      </c>
+      <c r="E117" t="s">
+        <v>5</v>
+      </c>
+      <c r="F117">
+        <f>F115*F113</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D118" t="s">
+        <v>6</v>
+      </c>
+      <c r="E118" t="s">
+        <v>7</v>
+      </c>
+      <c r="F118">
+        <f>F115-F116</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D119" t="s">
+        <v>8</v>
+      </c>
+      <c r="E119" t="s">
+        <v>9</v>
+      </c>
+      <c r="F119">
+        <f>F115-F118</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D120" t="s">
+        <v>10</v>
+      </c>
+      <c r="E120" t="s">
+        <v>12</v>
+      </c>
+      <c r="F120">
+        <f>F117/F118</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D121" t="s">
+        <v>11</v>
+      </c>
+      <c r="E121" t="s">
+        <v>13</v>
+      </c>
+      <c r="F121">
+        <f>F117/F119</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D122" t="s">
+        <v>14</v>
+      </c>
+      <c r="E122" t="s">
+        <v>15</v>
+      </c>
+      <c r="F122" s="1" t="b">
+        <f>IF(MOD(F117,F118)=0,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E123" t="s">
+        <v>16</v>
+      </c>
+      <c r="F123" s="1" t="b">
+        <f>IF(MOD(F117,F121)=0,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E124" t="s">
+        <v>18</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E125" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>